<commit_message>
Modifiqué el archivo de informe
</commit_message>
<xml_diff>
--- a/Informes/Informe_de_registro.xlsx
+++ b/Informes/Informe_de_registro.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\seminarioAlfa\regi03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repositorio_Grupal\Informes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B6BA65-E794-43A4-9B13-536690C20FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA6032DA-4E68-4F91-8CEF-7D3645D570BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>cod</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>dell</t>
+  </si>
+  <si>
+    <t>Asus</t>
   </si>
 </sst>
 </file>
@@ -84,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,56 +370,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1213</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>213</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>4231</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>23623</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>51441</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>56465147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>